<commit_message>
actualizacion actividades a 20 enero
</commit_message>
<xml_diff>
--- a/Horas Extra/2023/1.enero.xlsx
+++ b/Horas Extra/2023/1.enero.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="REPORTE HORAS EXTRAS" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>SISTEMA INTEGRADO DE GESTION</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Desarrollo de flujo AIC + PLC producidos y consumidos, emulando 3G para sistema Scada. Solución de problema de paro de VSD Mips 2500(proyectos) 18:00 a 22:00</t>
+  </si>
+  <si>
+    <t>Compensatorio</t>
   </si>
 </sst>
 </file>
@@ -1193,10 +1196,91 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="12" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="12" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1210,87 +1294,6 @@
     </xf>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1353,7 +1356,7 @@
         <xdr:cNvPr id="4" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1704,119 +1707,119 @@
   </sheetPr>
   <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B14" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11:L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="31.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="5" width="14" style="117" customWidth="1"/>
-    <col min="6" max="7" width="20.33203125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" style="104" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="31.44140625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="21.33203125" customWidth="1"/>
-    <col min="12" max="12" width="40.5546875" style="12" customWidth="1"/>
+    <col min="6" max="7" width="20.28515625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" style="104" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
+    <col min="12" max="12" width="40.5703125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="11.25" customHeight="1">
-      <c r="A1" s="125"/>
-      <c r="B1" s="126"/>
-      <c r="C1" s="142" t="s">
+      <c r="A1" s="119"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="143"/>
-      <c r="I1" s="143"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="136" t="s">
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="137"/>
+      <c r="L1" s="131"/>
     </row>
     <row r="2" spans="1:25" ht="11.25" customHeight="1">
-      <c r="A2" s="127"/>
-      <c r="B2" s="128"/>
-      <c r="C2" s="136"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
-      <c r="H2" s="145"/>
-      <c r="I2" s="145"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="137"/>
+      <c r="A2" s="121"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="139"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="139"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="130"/>
+      <c r="L2" s="131"/>
     </row>
     <row r="3" spans="1:25" ht="11.25" customHeight="1">
-      <c r="A3" s="127"/>
-      <c r="B3" s="128"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="145"/>
-      <c r="E3" s="145"/>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="145"/>
-      <c r="J3" s="137"/>
-      <c r="K3" s="136" t="s">
+      <c r="A3" s="121"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="139"/>
+      <c r="E3" s="139"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="139"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="137"/>
+      <c r="L3" s="131"/>
       <c r="N3" s="22"/>
     </row>
     <row r="4" spans="1:25" ht="11.25" customHeight="1">
-      <c r="A4" s="127"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="134" t="s">
+      <c r="A4" s="121"/>
+      <c r="B4" s="122"/>
+      <c r="C4" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="134"/>
-      <c r="G4" s="134"/>
-      <c r="H4" s="134"/>
-      <c r="I4" s="134"/>
-      <c r="J4" s="134"/>
-      <c r="K4" s="138"/>
-      <c r="L4" s="139"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
+      <c r="K4" s="132"/>
+      <c r="L4" s="133"/>
       <c r="N4" s="22"/>
     </row>
     <row r="5" spans="1:25" ht="11.25" customHeight="1">
-      <c r="A5" s="127"/>
-      <c r="B5" s="128"/>
-      <c r="C5" s="134"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="134"/>
-      <c r="F5" s="134"/>
-      <c r="G5" s="134"/>
-      <c r="H5" s="134"/>
-      <c r="I5" s="134"/>
-      <c r="J5" s="134"/>
-      <c r="K5" s="140" t="s">
+      <c r="A5" s="121"/>
+      <c r="B5" s="122"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="128"/>
+      <c r="K5" s="134" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="141"/>
+      <c r="L5" s="135"/>
     </row>
     <row r="6" spans="1:25" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A6" s="129"/>
-      <c r="B6" s="130"/>
-      <c r="C6" s="135"/>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="137"/>
+      <c r="A6" s="123"/>
+      <c r="B6" s="124"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="131"/>
     </row>
     <row r="7" spans="1:25" ht="6" customHeight="1" thickBot="1">
       <c r="A7" s="6"/>
@@ -1845,12 +1848,12 @@
       <c r="F8" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="51">
-        <v>1099218066</v>
-      </c>
+      <c r="G8" s="51"/>
       <c r="H8" s="92"/>
       <c r="I8" s="51"/>
-      <c r="J8" s="52"/>
+      <c r="J8" s="52">
+        <v>1099218066</v>
+      </c>
       <c r="K8" s="53" t="s">
         <v>3</v>
       </c>
@@ -1890,54 +1893,54 @@
       <c r="L10" s="60"/>
     </row>
     <row r="11" spans="1:25" ht="12.75" customHeight="1">
-      <c r="A11" s="131" t="s">
+      <c r="A11" s="125" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="119" t="s">
+      <c r="B11" s="142" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="119"/>
-      <c r="D11" s="148" t="s">
+      <c r="C11" s="142"/>
+      <c r="D11" s="144" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="148" t="s">
+      <c r="E11" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="146" t="s">
+      <c r="F11" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="146" t="s">
+      <c r="G11" s="140" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="148" t="s">
+      <c r="H11" s="144" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="119" t="s">
+      <c r="I11" s="142" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="119" t="s">
+      <c r="J11" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="146" t="s">
+      <c r="K11" s="140" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="150" t="s">
+      <c r="L11" s="146" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="12.75" customHeight="1">
-      <c r="A12" s="132"/>
-      <c r="B12" s="120"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="149"/>
-      <c r="E12" s="149"/>
-      <c r="F12" s="147"/>
-      <c r="G12" s="147"/>
-      <c r="H12" s="149"/>
-      <c r="I12" s="120"/>
-      <c r="J12" s="120"/>
-      <c r="K12" s="147"/>
-      <c r="L12" s="151"/>
+      <c r="A12" s="126"/>
+      <c r="B12" s="143"/>
+      <c r="C12" s="143"/>
+      <c r="D12" s="145"/>
+      <c r="E12" s="145"/>
+      <c r="F12" s="141"/>
+      <c r="G12" s="141"/>
+      <c r="H12" s="145"/>
+      <c r="I12" s="143"/>
+      <c r="J12" s="143"/>
+      <c r="K12" s="141"/>
+      <c r="L12" s="147"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1953,22 +1956,22 @@
       <c r="Y12" s="2"/>
     </row>
     <row r="13" spans="1:25" ht="22.5" customHeight="1">
-      <c r="A13" s="133"/>
+      <c r="A13" s="127"/>
       <c r="B13" s="48" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="149"/>
-      <c r="E13" s="149"/>
-      <c r="F13" s="147"/>
-      <c r="G13" s="147"/>
-      <c r="H13" s="149"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="147"/>
-      <c r="L13" s="151"/>
+      <c r="D13" s="145"/>
+      <c r="E13" s="145"/>
+      <c r="F13" s="141"/>
+      <c r="G13" s="141"/>
+      <c r="H13" s="145"/>
+      <c r="I13" s="143"/>
+      <c r="J13" s="143"/>
+      <c r="K13" s="141"/>
+      <c r="L13" s="147"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1993,9 +1996,7 @@
       <c r="C14" s="88">
         <v>0.20833333333333334</v>
       </c>
-      <c r="D14" s="89">
-        <v>8</v>
-      </c>
+      <c r="D14" s="89"/>
       <c r="E14" s="95"/>
       <c r="F14" s="85"/>
       <c r="G14" s="86"/>
@@ -2007,7 +2008,9 @@
       <c r="K14" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="L14" s="77"/>
+      <c r="L14" s="77" t="s">
+        <v>46</v>
+      </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -2102,7 +2105,7 @@
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="1:25" ht="74.55" customHeight="1">
+    <row r="17" spans="1:25" ht="74.650000000000006" customHeight="1">
       <c r="A17" s="83">
         <v>44934</v>
       </c>
@@ -2141,7 +2144,7 @@
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="1:25" ht="47.7" customHeight="1">
+    <row r="18" spans="1:25" ht="47.65" customHeight="1">
       <c r="A18" s="83">
         <v>44935</v>
       </c>
@@ -2182,7 +2185,7 @@
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
     </row>
-    <row r="19" spans="1:25" ht="63.45" customHeight="1">
+    <row r="19" spans="1:25" ht="63.4" customHeight="1">
       <c r="A19" s="82"/>
       <c r="B19" s="87"/>
       <c r="C19" s="88"/>
@@ -2209,7 +2212,7 @@
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" ht="58.95" customHeight="1">
+    <row r="20" spans="1:25" ht="58.9" customHeight="1">
       <c r="A20" s="21"/>
       <c r="B20" s="72"/>
       <c r="C20" s="73"/>
@@ -2263,7 +2266,7 @@
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
     </row>
-    <row r="22" spans="1:25" ht="37.200000000000003" customHeight="1">
+    <row r="22" spans="1:25" ht="37.15" customHeight="1">
       <c r="A22" s="21"/>
       <c r="B22" s="37"/>
       <c r="C22" s="38"/>
@@ -2317,7 +2320,7 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" ht="43.2" customHeight="1">
+    <row r="24" spans="1:25" ht="43.15" customHeight="1">
       <c r="A24" s="39"/>
       <c r="B24" s="37"/>
       <c r="C24" s="38"/>
@@ -2885,11 +2888,11 @@
       <c r="Y44" s="2"/>
     </row>
     <row r="45" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A45" s="122" t="s">
+      <c r="A45" s="149" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="123"/>
-      <c r="C45" s="124"/>
+      <c r="B45" s="150"/>
+      <c r="C45" s="151"/>
       <c r="D45" s="112">
         <f>SUM(D21:D44)</f>
         <v>0</v>
@@ -2931,12 +2934,12 @@
     <row r="47" spans="1:25" ht="24" customHeight="1">
       <c r="D47" s="113"/>
       <c r="E47" s="114"/>
-      <c r="F47" s="121"/>
-      <c r="G47" s="121"/>
-      <c r="H47" s="121"/>
-      <c r="I47" s="121"/>
-      <c r="J47" s="121"/>
-      <c r="K47" s="121"/>
+      <c r="F47" s="148"/>
+      <c r="G47" s="148"/>
+      <c r="H47" s="148"/>
+      <c r="I47" s="148"/>
+      <c r="J47" s="148"/>
+      <c r="K47" s="148"/>
       <c r="L47" s="16"/>
     </row>
     <row r="48" spans="1:25">
@@ -2955,11 +2958,11 @@
     </row>
     <row r="49" spans="1:13" ht="59.25" customHeight="1">
       <c r="A49" s="5"/>
-      <c r="B49" s="121"/>
-      <c r="C49" s="121"/>
+      <c r="B49" s="148"/>
+      <c r="C49" s="148"/>
       <c r="D49" s="115"/>
-      <c r="E49" s="121"/>
-      <c r="F49" s="121"/>
+      <c r="E49" s="148"/>
+      <c r="F49" s="148"/>
       <c r="G49" s="44"/>
       <c r="H49" s="102"/>
       <c r="I49" s="44"/>
@@ -2969,11 +2972,11 @@
       <c r="M49" s="3"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="B50" s="121"/>
-      <c r="C50" s="121"/>
+      <c r="B50" s="148"/>
+      <c r="C50" s="148"/>
       <c r="D50" s="116"/>
-      <c r="E50" s="121"/>
-      <c r="F50" s="121"/>
+      <c r="E50" s="148"/>
+      <c r="F50" s="148"/>
       <c r="G50" s="44"/>
       <c r="H50" s="102"/>
       <c r="I50" s="44"/>
@@ -2997,7 +3000,7 @@
       <c r="L51" s="14"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" ht="15.6">
+    <row r="52" spans="1:13" ht="15.75">
       <c r="A52" s="5"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
@@ -3012,7 +3015,7 @@
       <c r="L52" s="14"/>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13" ht="15.6">
+    <row r="53" spans="1:13" ht="15.75">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="116"/>
@@ -3057,6 +3060,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="F47:K47"/>
     <mergeCell ref="A1:B6"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="C4:J6"/>
@@ -3073,13 +3083,6 @@
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="G11:G13"/>
     <mergeCell ref="H11:H13"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="F47:K47"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -3100,16 +3103,16 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="43.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.8" thickBot="1"/>
-    <row r="2" spans="1:6" ht="15" thickBot="1">
+    <row r="1" spans="1:6" ht="13.5" thickBot="1"/>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="152" t="s">
         <v>24</v>
       </c>
@@ -3119,7 +3122,7 @@
       <c r="E2" s="153"/>
       <c r="F2" s="154"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="14.25">
       <c r="A3" s="155" t="s">
         <v>25</v>
       </c>
@@ -3133,7 +3136,7 @@
       <c r="E3" s="63"/>
       <c r="F3" s="63"/>
     </row>
-    <row r="4" spans="1:6" ht="27.6">
+    <row r="4" spans="1:6" ht="28.5">
       <c r="A4" s="156"/>
       <c r="B4" s="158"/>
       <c r="C4" s="158"/>

</xml_diff>